<commit_message>
instrTable update & Decode
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94A688A-9E6B-4467-9043-F7A1D6B6AA28}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4FA531-2EFE-4D9A-AE7D-81FBDBFA404C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="94">
   <si>
     <t>LUI</t>
   </si>
@@ -151,9 +151,6 @@
     <t>rd</t>
   </si>
   <si>
-    <t>upcode</t>
-  </si>
-  <si>
     <t>funct3</t>
   </si>
   <si>
@@ -278,6 +275,33 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>opcode</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>99</t>
   </si>
 </sst>
 </file>
@@ -345,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,6 +390,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -389,16 +419,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>434975</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>107553</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>148133</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>77049</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>59348</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>568181</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>51906</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -421,8 +451,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6573838" y="1603375"/>
-          <a:ext cx="6295286" cy="7685698"/>
+          <a:off x="10302280" y="1755477"/>
+          <a:ext cx="6287249" cy="7583304"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -433,14 +463,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>79175</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>304703</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>602359</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>156784</xdr:rowOff>
     </xdr:to>
@@ -465,8 +495,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6738937" y="0"/>
-          <a:ext cx="5710141" cy="1604584"/>
+          <a:off x="10921305" y="0"/>
+          <a:ext cx="5702402" cy="1585534"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -741,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="97" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="64" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -754,591 +784,678 @@
     <col min="3" max="5" width="9.06640625" style="1"/>
     <col min="6" max="6" width="16.06640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.53125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" style="8" customWidth="1"/>
     <col min="9" max="9" width="14.73046875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G14" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="E18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="E19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="E20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="E21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="E23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="E24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="E25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="E26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="E27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B37" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="G37" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B43" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -1347,10 +1464,10 @@
         <v>42</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -1359,10 +1476,13 @@
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="G44" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
@@ -1371,131 +1491,154 @@
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="G45" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B48" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B48" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="G48" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G56" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B57" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -1504,15 +1647,18 @@
         <v>42</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>